<commit_message>
Hyperparameter tweaks and testing results
</commit_message>
<xml_diff>
--- a/Dropout Automated Results.xlsx
+++ b/Dropout Automated Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darrick\Documents\Jupyter\senior-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8D4FEA-2924-46EE-8C55-7721CBBC270A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D8DA59-3FC6-4A17-9434-BD746FCC3CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{87FC1B79-4FA9-40D7-B3F5-59F08255F7DA}"/>
+    <workbookView xWindow="5115" yWindow="2385" windowWidth="21600" windowHeight="11385" xr2:uid="{87FC1B79-4FA9-40D7-B3F5-59F08255F7DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Epochs</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Dropout%</t>
+  </si>
+  <si>
+    <t>RMSE</t>
   </si>
 </sst>
 </file>
@@ -159,7 +162,86 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -321,44 +403,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <right style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
@@ -437,36 +481,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96E8BDAD-138C-44FD-B8A2-180463BE3F05}" name="Table1" displayName="Table1" ref="A1:H141" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:H141" xr:uid="{96E8BDAD-138C-44FD-B8A2-180463BE3F05}">
-    <filterColumn colId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96E8BDAD-138C-44FD-B8A2-180463BE3F05}" name="Table1" displayName="Table1" ref="A1:I141" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:I141" xr:uid="{96E8BDAD-138C-44FD-B8A2-180463BE3F05}">
+    <filterColumn colId="4">
       <filters>
-        <filter val="56.7070787"/>
-        <filter val="61.14585221"/>
+        <filter val="7.530410261"/>
+        <filter val="7.604830274"/>
+        <filter val="7.684042837"/>
+        <filter val="7.819581332"/>
+        <filter val="7.82488157"/>
+        <filter val="7.856300985"/>
+        <filter val="7.867840516"/>
+        <filter val="7.878491358"/>
+        <filter val="7.902523526"/>
+        <filter val="7.913586102"/>
+        <filter val="7.94124266"/>
+        <filter val="7.941337946"/>
+        <filter val="7.960141177"/>
+        <filter val="7.963437006"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="4">
+    <filterColumn colId="7">
       <filters>
-        <filter val="4.517501836"/>
-        <filter val="4.611918854"/>
-        <filter val="4.618497899"/>
-        <filter val="4.720859946"/>
-        <filter val="4.724124716"/>
-        <filter val="4.763478253"/>
-        <filter val="4.774888125"/>
-        <filter val="4.791602708"/>
+        <filter val="FALSE"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="2" xr3:uid="{12F791EE-0417-45A8-A585-7BFB516070F1}" name="Dropout%"/>
     <tableColumn id="3" xr3:uid="{FD837FEA-1BA9-4E3A-B16D-0068E2237A3D}" name="Batch"/>
-    <tableColumn id="4" xr3:uid="{6118DEA7-2AC1-4DFB-93DE-61FFC04C3D71}" name="Epochs" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{8D7D2041-99F1-4790-9C24-EC59FC9512B4}" name="Loss" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{6B513DFC-D100-42C7-AB37-594EEC1E8E85}" name="50th Quantile" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{5032E873-4C59-4027-88EB-566783F747A2}" name="%Accept" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{080111E8-9AD5-415A-BDE1-8022C60387B7}" name="Overfit" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{363CCBD0-646F-4D96-A60A-D383E01D85DA}" name="Notes" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{6118DEA7-2AC1-4DFB-93DE-61FFC04C3D71}" name="Epochs" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{8D7D2041-99F1-4790-9C24-EC59FC9512B4}" name="Loss" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{3FC93D8E-C47D-4E8F-BDB0-2FE9B5A21554}" name="RMSE" dataDxfId="0">
+      <calculatedColumnFormula>SQRT(Table1[[#This Row],[Loss]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{6B513DFC-D100-42C7-AB37-594EEC1E8E85}" name="50th Quantile" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{5032E873-4C59-4027-88EB-566783F747A2}" name="%Accept" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{080111E8-9AD5-415A-BDE1-8022C60387B7}" name="Overfit" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{363CCBD0-646F-4D96-A60A-D383E01D85DA}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -769,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30900C23-159C-4CAB-B086-0C779BA0E7B7}">
-  <dimension ref="A1:H141"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G144" sqref="G144"/>
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,7 +838,7 @@
     <col min="8" max="8" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -800,19 +852,22 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.3</v>
       </c>
@@ -826,17 +881,21 @@
         <v>65.656766972568207</v>
       </c>
       <c r="E2" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.1028863359032872</v>
+      </c>
+      <c r="F2" s="4">
         <v>5.1828885513549601</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>48.983364140480496</v>
       </c>
-      <c r="G2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.3</v>
       </c>
@@ -850,17 +909,21 @@
         <v>79.5532122768888</v>
       </c>
       <c r="E3" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.9192607472194023</v>
+      </c>
+      <c r="F3" s="4">
         <v>5.4719598395972602</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>45.656192236598798</v>
       </c>
-      <c r="G3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -874,17 +937,21 @@
         <v>79.480408913547095</v>
       </c>
       <c r="E4" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.9151785687975487</v>
+      </c>
+      <c r="F4" s="4">
         <v>5.3313751977962998</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>47.504621072088703</v>
       </c>
-      <c r="G4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.3</v>
       </c>
@@ -898,17 +965,21 @@
         <v>87.964622483456196</v>
       </c>
       <c r="E5" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.3789457021275151</v>
+      </c>
+      <c r="F5" s="4">
         <v>5.7935174018023599</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>45.471349353049902</v>
       </c>
-      <c r="G5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.3</v>
       </c>
@@ -922,17 +993,21 @@
         <v>62.449878072121599</v>
       </c>
       <c r="E6" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.9025235255658428</v>
+      </c>
+      <c r="F6" s="4">
         <v>5.0124395283639496</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>49.7227356746765</v>
       </c>
-      <c r="G6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.3</v>
       </c>
@@ -946,17 +1021,21 @@
         <v>67.831373401578304</v>
       </c>
       <c r="E7" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2359804153226541</v>
+      </c>
+      <c r="F7" s="4">
         <v>5.2243075088173798</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>46.580406654343797</v>
       </c>
-      <c r="G7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.3</v>
       </c>
@@ -970,17 +1049,21 @@
         <v>69.650231768595702</v>
       </c>
       <c r="E8" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3456714390512463</v>
+      </c>
+      <c r="F8" s="4">
         <v>5.3199205098883704</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <v>47.689463955637699</v>
       </c>
-      <c r="G8" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.3</v>
       </c>
@@ -994,17 +1077,21 @@
         <v>82.012219808017903</v>
       </c>
       <c r="E9" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.0560598390259059</v>
+      </c>
+      <c r="F9" s="4">
         <v>5.1806662489728197</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>47.874306839186602</v>
       </c>
-      <c r="G9" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.3</v>
       </c>
@@ -1018,17 +1105,21 @@
         <v>70.666888936830702</v>
       </c>
       <c r="E10" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.4063600289798863</v>
+      </c>
+      <c r="F10" s="4">
         <v>5.7121406465568798</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>44.731977818853899</v>
       </c>
-      <c r="G10" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.3</v>
       </c>
@@ -1042,17 +1133,21 @@
         <v>67.098156419567104</v>
       </c>
       <c r="E11" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.1913464350842293</v>
+      </c>
+      <c r="F11" s="4">
         <v>4.9827571807097204</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <v>50.277264325323401</v>
       </c>
-      <c r="G11" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.3</v>
       </c>
@@ -1066,17 +1161,21 @@
         <v>69.376923143312794</v>
       </c>
       <c r="E12" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3292810700151545</v>
+      </c>
+      <c r="F12" s="4">
         <v>5.4335343043009399</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <v>46.580406654343797</v>
       </c>
-      <c r="G12" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.3</v>
       </c>
@@ -1090,17 +1189,21 @@
         <v>89.093914010828797</v>
       </c>
       <c r="E13" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.4389572523043448</v>
+      </c>
+      <c r="F13" s="4">
         <v>5.5510685005966396</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="4">
         <v>44.916820702402902</v>
       </c>
-      <c r="G13" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.3</v>
       </c>
@@ -1114,17 +1217,21 @@
         <v>77.139974809177701</v>
       </c>
       <c r="E14" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.7829365709412759</v>
+      </c>
+      <c r="F14" s="4">
         <v>5.6266847009212801</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G14" s="4">
         <v>44.731977818853899</v>
       </c>
-      <c r="G14" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.3</v>
       </c>
@@ -1138,17 +1245,21 @@
         <v>64.580948482379398</v>
       </c>
       <c r="E15" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0362272542766853</v>
+      </c>
+      <c r="F15" s="4">
         <v>4.8242239798268898</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="4">
         <v>51.2014787430683</v>
       </c>
-      <c r="G15" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.3</v>
       </c>
@@ -1162,17 +1273,21 @@
         <v>73.891427101798001</v>
       </c>
       <c r="E16" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5960122790627747</v>
+      </c>
+      <c r="F16" s="4">
         <v>5.3599571488861297</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
         <v>46.7652495378927</v>
       </c>
-      <c r="G16" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.3</v>
       </c>
@@ -1186,17 +1301,21 @@
         <v>81.350575459422103</v>
       </c>
       <c r="E17" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.019455385965502</v>
+      </c>
+      <c r="F17" s="4">
         <v>5.58995200847757</v>
       </c>
-      <c r="F17" s="4">
+      <c r="G17" s="4">
         <v>46.395563770794801</v>
       </c>
-      <c r="G17" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.3</v>
       </c>
@@ -1210,17 +1329,21 @@
         <v>66.033119624731896</v>
       </c>
       <c r="E18" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.1260765209744292</v>
+      </c>
+      <c r="F18" s="4">
         <v>5.4459652549889199</v>
       </c>
-      <c r="F18" s="4">
+      <c r="G18" s="4">
         <v>45.471349353049902</v>
       </c>
-      <c r="G18" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.3</v>
       </c>
@@ -1234,17 +1357,21 @@
         <v>73.522273601313401</v>
       </c>
       <c r="E19" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5745130241497325</v>
+      </c>
+      <c r="F19" s="4">
         <v>5.4881886344784903</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
         <v>46.210720887245799</v>
       </c>
-      <c r="G19" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.3</v>
       </c>
@@ -1258,17 +1385,21 @@
         <v>74.613442715346906</v>
       </c>
       <c r="E20" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.6379073111111175</v>
+      </c>
+      <c r="F20" s="4">
         <v>5.2311296141316204</v>
       </c>
-      <c r="F20" s="4">
+      <c r="G20" s="4">
         <v>48.2439926062846</v>
       </c>
-      <c r="G20" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.3</v>
       </c>
@@ -1282,17 +1413,21 @@
         <v>76.7066516840964</v>
       </c>
       <c r="E21" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.7582333654736786</v>
+      </c>
+      <c r="F21" s="4">
         <v>5.5523251061885599</v>
       </c>
-      <c r="F21" s="4">
+      <c r="G21" s="4">
         <v>46.025878003696803</v>
       </c>
-      <c r="G21" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.4</v>
       </c>
@@ -1306,17 +1441,21 @@
         <v>68.670749699562606</v>
       </c>
       <c r="E22" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2867816249472028</v>
+      </c>
+      <c r="F22" s="4">
         <v>4.8501197729217802</v>
       </c>
-      <c r="F22" s="4">
+      <c r="G22" s="4">
         <v>52.310536044362202</v>
       </c>
-      <c r="G22" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.4</v>
       </c>
@@ -1330,17 +1469,21 @@
         <v>73.621935564136294</v>
       </c>
       <c r="E23" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5803225792586773</v>
+      </c>
+      <c r="F23" s="4">
         <v>5.1963500379583198</v>
       </c>
-      <c r="F23" s="4">
+      <c r="G23" s="4">
         <v>48.2439926062846</v>
       </c>
-      <c r="G23" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.4</v>
       </c>
@@ -1354,17 +1497,21 @@
         <v>71.393382603051194</v>
       </c>
       <c r="E24" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.4494604918332623</v>
+      </c>
+      <c r="F24" s="4">
         <v>5.37840555959363</v>
       </c>
-      <c r="F24" s="4">
+      <c r="G24" s="4">
         <v>47.319778188539701</v>
       </c>
-      <c r="G24" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.4</v>
       </c>
@@ -1378,17 +1525,21 @@
         <v>72.308898502709397</v>
       </c>
       <c r="E25" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5034639120013562</v>
+      </c>
+      <c r="F25" s="4">
         <v>5.5615849688770203</v>
       </c>
-      <c r="F25" s="4">
+      <c r="G25" s="4">
         <v>46.210720887245799</v>
       </c>
-      <c r="G25" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.4</v>
       </c>
@@ -1402,17 +1553,21 @@
         <v>71.624423578794605</v>
       </c>
       <c r="E26" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.4631213850915916</v>
+      </c>
+      <c r="F26" s="4">
         <v>4.98325321772327</v>
       </c>
-      <c r="F26" s="4">
+      <c r="G26" s="4">
         <v>50.646950092421399</v>
       </c>
-      <c r="G26" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.4</v>
       </c>
@@ -1426,17 +1581,21 @@
         <v>67.889691816460399</v>
       </c>
       <c r="E27" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2395201205203943</v>
+      </c>
+      <c r="F27" s="4">
         <v>5.0303567841995598</v>
       </c>
-      <c r="F27" s="4">
+      <c r="G27" s="4">
         <v>49.7227356746765</v>
       </c>
-      <c r="G27" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.4</v>
       </c>
@@ -1450,17 +1609,21 @@
         <v>70.938843732400201</v>
       </c>
       <c r="E28" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.4225200345502422</v>
+      </c>
+      <c r="F28" s="4">
         <v>5.5665827586640804</v>
       </c>
-      <c r="F28" s="4">
+      <c r="G28" s="4">
         <v>45.471349353049902</v>
       </c>
-      <c r="G28" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.4</v>
       </c>
@@ -1474,17 +1637,21 @@
         <v>87.286272595417898</v>
       </c>
       <c r="E29" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.3427122718950244</v>
+      </c>
+      <c r="F29" s="4">
         <v>6.1235127965509104</v>
       </c>
-      <c r="F29" s="4">
+      <c r="G29" s="4">
         <v>43.622920517559997</v>
       </c>
-      <c r="G29" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.4</v>
       </c>
@@ -1498,17 +1665,21 @@
         <v>69.181338156878098</v>
       </c>
       <c r="E30" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3175319751040391</v>
+      </c>
+      <c r="F30" s="4">
         <v>5.5781353929733699</v>
       </c>
-      <c r="F30" s="4">
+      <c r="G30" s="4">
         <v>44.916820702402902</v>
       </c>
-      <c r="G30" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.4</v>
       </c>
@@ -1522,17 +1693,21 @@
         <v>65.904782088979502</v>
       </c>
       <c r="E31" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.1181760321502949</v>
+      </c>
+      <c r="F31" s="4">
         <v>5.2439418780766296</v>
       </c>
-      <c r="F31" s="4">
+      <c r="G31" s="4">
         <v>47.504621072088703</v>
       </c>
-      <c r="G31" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.4</v>
       </c>
@@ -1546,17 +1721,21 @@
         <v>69.264562490466702</v>
       </c>
       <c r="E32" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3225334178041432</v>
+      </c>
+      <c r="F32" s="4">
         <v>5.0640410061540297</v>
       </c>
-      <c r="F32" s="4">
+      <c r="G32" s="4">
         <v>49.353049907578502</v>
       </c>
-      <c r="G32" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.4</v>
       </c>
@@ -1570,17 +1749,21 @@
         <v>82.194779725700499</v>
       </c>
       <c r="E33" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.0661336701871154</v>
+      </c>
+      <c r="F33" s="4">
         <v>5.7827432126093701</v>
       </c>
-      <c r="F33" s="4">
+      <c r="G33" s="4">
         <v>43.992606284658002</v>
       </c>
-      <c r="G33" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.4</v>
       </c>
@@ -1594,17 +1777,21 @@
         <v>65.501421267356093</v>
       </c>
       <c r="E34" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0932948338335038</v>
+      </c>
+      <c r="F34" s="4">
         <v>5.42321209947601</v>
       </c>
-      <c r="F34" s="4">
+      <c r="G34" s="4">
         <v>46.950092421441703</v>
       </c>
-      <c r="G34" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.4</v>
       </c>
@@ -1618,17 +1805,21 @@
         <v>74.080225241162196</v>
       </c>
       <c r="E35" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.6069870013357281</v>
+      </c>
+      <c r="F35" s="4">
         <v>5.0992651128912101</v>
       </c>
-      <c r="F35" s="4">
+      <c r="G35" s="4">
         <v>48.983364140480496</v>
       </c>
-      <c r="G35" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.4</v>
       </c>
@@ -1642,17 +1833,21 @@
         <v>75.760046389539198</v>
       </c>
       <c r="E36" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.7040247236286739</v>
+      </c>
+      <c r="F36" s="4">
         <v>5.4209132994581299</v>
       </c>
-      <c r="F36" s="4">
+      <c r="G36" s="4">
         <v>47.134935304990698</v>
       </c>
-      <c r="G36" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.4</v>
       </c>
@@ -1666,17 +1861,21 @@
         <v>76.700422953325301</v>
       </c>
       <c r="E37" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.7578777653793107</v>
+      </c>
+      <c r="F37" s="4">
         <v>5.4740594156672397</v>
       </c>
-      <c r="F37" s="4">
+      <c r="G37" s="4">
         <v>46.025878003696803</v>
       </c>
-      <c r="G37" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.4</v>
       </c>
@@ -1690,17 +1889,21 @@
         <v>82.423941437726498</v>
       </c>
       <c r="E38" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.0787632107973</v>
+      </c>
+      <c r="F38" s="4">
         <v>5.7166689823936698</v>
       </c>
-      <c r="F38" s="4">
+      <c r="G38" s="4">
         <v>44.916820702402902</v>
       </c>
-      <c r="G38" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.4</v>
       </c>
@@ -1714,17 +1917,21 @@
         <v>68.255384364101602</v>
       </c>
       <c r="E39" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2616816910421811</v>
+      </c>
+      <c r="F39" s="4">
         <v>5.0853937354672798</v>
       </c>
-      <c r="F39" s="4">
+      <c r="G39" s="4">
         <v>49.353049907578502</v>
       </c>
-      <c r="G39" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.4</v>
       </c>
@@ -1738,17 +1945,21 @@
         <v>82.421406264666402</v>
       </c>
       <c r="E40" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.078623588665101</v>
+      </c>
+      <c r="F40" s="4">
         <v>5.5515104353185896</v>
       </c>
-      <c r="F40" s="4">
+      <c r="G40" s="4">
         <v>46.580406654343797</v>
       </c>
-      <c r="G40" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.4</v>
       </c>
@@ -1762,17 +1973,21 @@
         <v>66.320862465116306</v>
       </c>
       <c r="E41" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.1437621812720131</v>
+      </c>
+      <c r="F41" s="4">
         <v>5.56954985398513</v>
       </c>
-      <c r="F41" s="4">
+      <c r="G41" s="4">
         <v>45.2865064695009</v>
       </c>
-      <c r="G41" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.5</v>
       </c>
@@ -1786,17 +2001,21 @@
         <v>72.305555579843002</v>
       </c>
       <c r="E42" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5032673473108566</v>
+      </c>
+      <c r="F42" s="4">
         <v>5.3022690510404296</v>
       </c>
-      <c r="F42" s="4">
+      <c r="G42" s="4">
         <v>48.983364140480496</v>
       </c>
-      <c r="G42" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.5</v>
       </c>
@@ -1810,17 +2029,21 @@
         <v>70.177193562336598</v>
       </c>
       <c r="E43" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3771829132672391</v>
+      </c>
+      <c r="F43" s="4">
         <v>5.4125096328615196</v>
       </c>
-      <c r="F43" s="4">
+      <c r="G43" s="4">
         <v>46.950092421441703</v>
       </c>
-      <c r="G43" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.5</v>
       </c>
@@ -1834,17 +2057,21 @@
         <v>66.513115013813504</v>
       </c>
       <c r="E44" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.1555573085972188</v>
+      </c>
+      <c r="F44" s="4">
         <v>5.16505863355553</v>
       </c>
-      <c r="F44" s="4">
+      <c r="G44" s="4">
         <v>49.168207024029499</v>
       </c>
-      <c r="G44" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.5</v>
       </c>
@@ -1858,17 +2085,21 @@
         <v>80.9798871250117</v>
       </c>
       <c r="E45" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.9988825486841257</v>
+      </c>
+      <c r="F45" s="4">
         <v>5.3955419673476097</v>
       </c>
-      <c r="F45" s="4">
+      <c r="G45" s="4">
         <v>45.656192236598798</v>
       </c>
-      <c r="G45" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.5</v>
       </c>
@@ -1882,17 +2113,21 @@
         <v>74.658220795298206</v>
       </c>
       <c r="E46" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.6404988742142788</v>
+      </c>
+      <c r="F46" s="4">
         <v>4.8296222686767498</v>
       </c>
-      <c r="F46" s="4">
+      <c r="G46" s="4">
         <v>51.386321626617303</v>
       </c>
-      <c r="G46" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H46" s="4"/>
-    </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.5</v>
       </c>
@@ -1906,17 +2141,21 @@
         <v>63.416328955489902</v>
       </c>
       <c r="E47" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.9634370064369762</v>
+      </c>
+      <c r="F47" s="4">
         <v>5.3576068119030102</v>
       </c>
-      <c r="F47" s="4">
+      <c r="G47" s="4">
         <v>48.2439926062846</v>
       </c>
-      <c r="G47" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.5</v>
       </c>
@@ -1930,17 +2169,21 @@
         <v>69.967659419653799</v>
       </c>
       <c r="E48" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.364667322712469</v>
+      </c>
+      <c r="F48" s="4">
         <v>5.1344351485878903</v>
       </c>
-      <c r="F48" s="4">
+      <c r="G48" s="4">
         <v>48.983364140480496</v>
       </c>
-      <c r="G48" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.5</v>
       </c>
@@ -1954,17 +2197,21 @@
         <v>67.418515034391703</v>
       </c>
       <c r="E49" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2108778479765299</v>
+      </c>
+      <c r="F49" s="4">
         <v>5.0868393345223604</v>
       </c>
-      <c r="F49" s="4">
+      <c r="G49" s="4">
         <v>49.353049907578502</v>
       </c>
-      <c r="G49" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.5</v>
       </c>
@@ -1978,17 +2225,21 @@
         <v>64.632834274094506</v>
       </c>
       <c r="E50" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.039454849310026</v>
+      </c>
+      <c r="F50" s="4">
         <v>4.9493221067032698</v>
       </c>
-      <c r="F50" s="4">
+      <c r="G50" s="4">
         <v>50.092421441774398</v>
       </c>
-      <c r="G50" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0.5</v>
       </c>
@@ -2002,17 +2253,21 @@
         <v>63.493529547164201</v>
       </c>
       <c r="E51" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.9682827225923782</v>
+      </c>
+      <c r="F51" s="4">
         <v>5.2023141500833097</v>
       </c>
-      <c r="F51" s="4">
+      <c r="G51" s="4">
         <v>48.983364140480496</v>
       </c>
-      <c r="G51" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H51" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0.5</v>
       </c>
@@ -2026,17 +2281,21 @@
         <v>69.127414738625106</v>
       </c>
       <c r="E52" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3142897915952574</v>
+      </c>
+      <c r="F52" s="4">
         <v>5.1796514809536998</v>
       </c>
-      <c r="F52" s="4">
+      <c r="G52" s="4">
         <v>48.7985212569316</v>
       </c>
-      <c r="G52" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0.5</v>
       </c>
@@ -2050,17 +2309,21 @@
         <v>74.495134152678602</v>
       </c>
       <c r="E53" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.6310563752462315</v>
+      </c>
+      <c r="F53" s="4">
         <v>5.8261359902315304</v>
       </c>
-      <c r="F53" s="4">
+      <c r="G53" s="4">
         <v>45.2865064695009</v>
       </c>
-      <c r="G53" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H53" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0.5</v>
       </c>
@@ -2074,17 +2337,21 @@
         <v>64.703852662317402</v>
       </c>
       <c r="E54" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0438705025825357</v>
+      </c>
+      <c r="F54" s="4">
         <v>4.9199891771589002</v>
       </c>
-      <c r="F54" s="4">
+      <c r="G54" s="4">
         <v>50.462107208872403</v>
       </c>
-      <c r="G54" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H54" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0.5</v>
       </c>
@@ -2098,17 +2365,21 @@
         <v>61.145852214086901</v>
       </c>
       <c r="E55" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.8195813324043701</v>
+      </c>
+      <c r="F55" s="4">
         <v>4.5175018356562404</v>
       </c>
-      <c r="F55" s="4">
+      <c r="G55" s="4">
         <v>53.789279112754102</v>
       </c>
-      <c r="G55" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0.5</v>
       </c>
@@ -2122,17 +2393,21 @@
         <v>63.064848379815501</v>
       </c>
       <c r="E56" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.9413379464555911</v>
+      </c>
+      <c r="F56" s="4">
         <v>5.2777727300470501</v>
       </c>
-      <c r="F56" s="4">
+      <c r="G56" s="4">
         <v>49.168207024029499</v>
       </c>
-      <c r="G56" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H56" s="4"/>
-    </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0.5</v>
       </c>
@@ -2146,17 +2421,21 @@
         <v>68.362844893760396</v>
       </c>
       <c r="E57" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.268182683864719</v>
+      </c>
+      <c r="F57" s="4">
         <v>4.9919688606708803</v>
       </c>
-      <c r="F57" s="4">
+      <c r="G57" s="4">
         <v>50.092421441774398</v>
       </c>
-      <c r="G57" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H57" s="4"/>
-    </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H57" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0.5</v>
       </c>
@@ -2170,17 +2449,21 @@
         <v>70.450678742526804</v>
       </c>
       <c r="E58" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3934902598696564</v>
+      </c>
+      <c r="F58" s="4">
         <v>4.9686932961535897</v>
       </c>
-      <c r="F58" s="4">
+      <c r="G58" s="4">
         <v>50.277264325323401</v>
       </c>
-      <c r="G58" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H58" s="4"/>
-    </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H58" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0.5</v>
       </c>
@@ -2194,17 +2477,21 @@
         <v>67.403177412953198</v>
       </c>
       <c r="E59" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2099438130204767</v>
+      </c>
+      <c r="F59" s="4">
         <v>5.1211734440015704</v>
       </c>
-      <c r="F59" s="4">
+      <c r="G59" s="4">
         <v>49.353049907578502</v>
       </c>
-      <c r="G59" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H59" s="4"/>
-    </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H59" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>0.5</v>
       </c>
@@ -2218,17 +2505,21 @@
         <v>70.6330372498348</v>
       </c>
       <c r="E60" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.4043463309072877</v>
+      </c>
+      <c r="F60" s="4">
         <v>5.1376048357058703</v>
       </c>
-      <c r="F60" s="4">
+      <c r="G60" s="4">
         <v>49.168207024029499</v>
       </c>
-      <c r="G60" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H60" s="4"/>
-    </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H60" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0.5</v>
       </c>
@@ -2242,17 +2533,21 @@
         <v>73.207939049232394</v>
       </c>
       <c r="E61" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5561638044881061</v>
+      </c>
+      <c r="F61" s="4">
         <v>5.3817167017603103</v>
       </c>
-      <c r="F61" s="4">
+      <c r="G61" s="4">
         <v>47.874306839186602</v>
       </c>
-      <c r="G61" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H61" s="4"/>
-    </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H61" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0.6</v>
       </c>
@@ -2266,17 +2561,21 @@
         <v>70.191514528172206</v>
       </c>
       <c r="E62" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3780376299090591</v>
+      </c>
+      <c r="F62" s="4">
         <v>4.8611175196436296</v>
       </c>
-      <c r="F62" s="4">
+      <c r="G62" s="4">
         <v>51.940850277264303</v>
       </c>
-      <c r="G62" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H62" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0.6</v>
       </c>
@@ -2290,17 +2589,21 @@
         <v>64.638222241357596</v>
       </c>
       <c r="E63" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0397899376387691</v>
+      </c>
+      <c r="F63" s="4">
         <v>5.0230007956888096</v>
       </c>
-      <c r="F63" s="4">
+      <c r="G63" s="4">
         <v>49.537892791127497</v>
       </c>
-      <c r="G63" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H63" s="4"/>
-    </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H63" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0.6</v>
       </c>
@@ -2314,17 +2617,21 @@
         <v>70.066269548454898</v>
       </c>
       <c r="E64" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3705596914695555</v>
+      </c>
+      <c r="F64" s="4">
         <v>4.9559290770775704</v>
       </c>
-      <c r="F64" s="4">
+      <c r="G64" s="4">
         <v>50.277264325323401</v>
       </c>
-      <c r="G64" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H64" s="4"/>
-    </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H64" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0.6</v>
       </c>
@@ -2338,17 +2645,21 @@
         <v>68.1215261082111</v>
       </c>
       <c r="E65" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2535765646300945</v>
+      </c>
+      <c r="F65" s="4">
         <v>5.4159866217105499</v>
       </c>
-      <c r="F65" s="4">
+      <c r="G65" s="4">
         <v>46.210720887245799</v>
       </c>
-      <c r="G65" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H65" s="4"/>
-    </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H65" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0.6</v>
       </c>
@@ -2362,17 +2673,21 @@
         <v>70.656361183265204</v>
       </c>
       <c r="E66" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.4057338277669249</v>
+      </c>
+      <c r="F66" s="4">
         <v>5.1959117866424096</v>
       </c>
-      <c r="F66" s="4">
+      <c r="G66" s="4">
         <v>47.874306839186602</v>
       </c>
-      <c r="G66" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H66" s="4"/>
-    </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H66" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0.6</v>
       </c>
@@ -2386,17 +2701,21 @@
         <v>64.9676169291441</v>
       </c>
       <c r="E67" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0602491853009166</v>
+      </c>
+      <c r="F67" s="4">
         <v>5.0510034788609302</v>
       </c>
-      <c r="F67" s="4">
+      <c r="G67" s="4">
         <v>49.537892791127497</v>
       </c>
-      <c r="G67" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H67" s="4"/>
-    </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H67" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I67" s="4"/>
+    </row>
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0.6</v>
       </c>
@@ -2410,17 +2729,21 @@
         <v>74.459256015291004</v>
       </c>
       <c r="E68" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.6289776923625787</v>
+      </c>
+      <c r="F68" s="4">
         <v>5.1776886677396403</v>
       </c>
-      <c r="F68" s="4">
+      <c r="G68" s="4">
         <v>48.2439926062846</v>
       </c>
-      <c r="G68" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H68" s="4"/>
-    </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H68" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68" s="4"/>
+    </row>
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0.6</v>
       </c>
@@ -2434,17 +2757,21 @@
         <v>66.555691801906704</v>
       </c>
       <c r="E69" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.1581671839884908</v>
+      </c>
+      <c r="F69" s="4">
         <v>5.2333226762652201</v>
       </c>
-      <c r="F69" s="4">
+      <c r="G69" s="4">
         <v>47.134935304990698</v>
       </c>
-      <c r="G69" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H69" s="4"/>
-    </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H69" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0.6</v>
       </c>
@@ -2458,17 +2785,21 @@
         <v>77.148666938880396</v>
       </c>
       <c r="E70" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.7834313874977354</v>
+      </c>
+      <c r="F70" s="4">
         <v>5.5477976819833801</v>
       </c>
-      <c r="F70" s="4">
+      <c r="G70" s="4">
         <v>43.992606284658002</v>
       </c>
-      <c r="G70" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H70" s="4"/>
-    </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H70" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I70" s="4"/>
+    </row>
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0.6</v>
       </c>
@@ -2482,17 +2813,21 @@
         <v>67.561851649539904</v>
       </c>
       <c r="E71" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2196016721943348</v>
+      </c>
+      <c r="F71" s="4">
         <v>4.7916027080616503</v>
       </c>
-      <c r="F71" s="4">
+      <c r="G71" s="4">
         <v>51.756007393715301</v>
       </c>
-      <c r="G71" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H71" s="4"/>
-    </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H71" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I71" s="4"/>
+    </row>
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0.6</v>
       </c>
@@ -2506,17 +2841,21 @@
         <v>69.478986038518201</v>
       </c>
       <c r="E72" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3354055713275397</v>
+      </c>
+      <c r="F72" s="4">
         <v>5.5071962892619597</v>
       </c>
-      <c r="F72" s="4">
+      <c r="G72" s="4">
         <v>45.101663585951897</v>
       </c>
-      <c r="G72" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H72" s="4"/>
-    </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H72" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I72" s="4"/>
+    </row>
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0.6</v>
       </c>
@@ -2530,17 +2869,21 @@
         <v>75.1682107188565</v>
       </c>
       <c r="E73" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.6699602489778744</v>
+      </c>
+      <c r="F73" s="4">
         <v>5.5872512346847403</v>
       </c>
-      <c r="F73" s="4">
+      <c r="G73" s="4">
         <v>46.025878003696803</v>
       </c>
-      <c r="G73" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H73" s="4"/>
-    </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H73" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I73" s="4"/>
+    </row>
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0.6</v>
       </c>
@@ -2554,17 +2897,21 @@
         <v>81.038733928349004</v>
       </c>
       <c r="E74" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.002151627713733</v>
+      </c>
+      <c r="F74" s="4">
         <v>5.3075823339971997</v>
       </c>
-      <c r="F74" s="4">
+      <c r="G74" s="4">
         <v>47.689463955637699</v>
       </c>
-      <c r="G74" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H74" s="4"/>
-    </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H74" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I74" s="4"/>
+    </row>
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0.6</v>
       </c>
@@ -2578,17 +2925,21 @@
         <v>65.311789845803304</v>
       </c>
       <c r="E75" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0815710010989381</v>
+      </c>
+      <c r="F75" s="4">
         <v>5.2741225763415596</v>
       </c>
-      <c r="F75" s="4">
+      <c r="G75" s="4">
         <v>48.2439926062846</v>
       </c>
-      <c r="G75" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H75" s="4"/>
-    </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H75" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I75" s="4"/>
+    </row>
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0.6</v>
       </c>
@@ -2602,17 +2953,21 @@
         <v>68.003706898574606</v>
       </c>
       <c r="E76" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.246436011912941</v>
+      </c>
+      <c r="F76" s="4">
         <v>5.1535087659640997</v>
       </c>
-      <c r="F76" s="4">
+      <c r="G76" s="4">
         <v>48.2439926062846</v>
       </c>
-      <c r="G76" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H76" s="4"/>
-    </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H76" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I76" s="4"/>
+    </row>
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0.6</v>
       </c>
@@ -2626,17 +2981,21 @@
         <v>73.225667096770806</v>
       </c>
       <c r="E77" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5571997228515588</v>
+      </c>
+      <c r="F77" s="4">
         <v>5.2533002334838699</v>
       </c>
-      <c r="F77" s="4">
+      <c r="G77" s="4">
         <v>47.319778188539701</v>
       </c>
-      <c r="G77" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H77" s="4"/>
-    </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H77" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I77" s="4"/>
+    </row>
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0.6</v>
       </c>
@@ -2650,17 +3009,21 @@
         <v>67.559269000774293</v>
       </c>
       <c r="E78" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2194445676562768</v>
+      </c>
+      <c r="F78" s="4">
         <v>5.0878303496174802</v>
       </c>
-      <c r="F78" s="4">
+      <c r="G78" s="4">
         <v>48.7985212569316</v>
       </c>
-      <c r="G78" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H78" s="4"/>
-    </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H78" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I78" s="4"/>
+    </row>
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0.6</v>
       </c>
@@ -2674,17 +3037,21 @@
         <v>67.434385246798598</v>
       </c>
       <c r="E79" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2118442049760425</v>
+      </c>
+      <c r="F79" s="4">
         <v>5.3229612622942204</v>
       </c>
-      <c r="F79" s="4">
+      <c r="G79" s="4">
         <v>47.874306839186602</v>
       </c>
-      <c r="G79" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H79" s="4"/>
-    </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H79" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I79" s="4"/>
+    </row>
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0.6</v>
       </c>
@@ -2698,17 +3065,21 @@
         <v>72.305629229589599</v>
       </c>
       <c r="E80" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5032716779831041</v>
+      </c>
+      <c r="F80" s="4">
         <v>5.8316459655761701</v>
       </c>
-      <c r="F80" s="4">
+      <c r="G80" s="4">
         <v>44.731977818853899</v>
       </c>
-      <c r="G80" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H80" s="4"/>
-    </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H80" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I80" s="4"/>
+    </row>
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0.6</v>
       </c>
@@ -2722,17 +3093,21 @@
         <v>67.560781778557597</v>
       </c>
       <c r="E81" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2195365914726359</v>
+      </c>
+      <c r="F81" s="4">
         <v>5.3518230460606002</v>
       </c>
-      <c r="F81" s="4">
+      <c r="G81" s="4">
         <v>46.950092421441703</v>
       </c>
-      <c r="G81" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H81" s="4"/>
-    </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H81" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I81" s="4"/>
+    </row>
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0.7</v>
       </c>
@@ -2746,17 +3121,21 @@
         <v>67.563636356713303</v>
       </c>
       <c r="E82" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2197102355687282</v>
+      </c>
+      <c r="F82" s="4">
         <v>4.7998542242513302</v>
       </c>
-      <c r="F82" s="4">
+      <c r="G82" s="4">
         <v>52.6802218114602</v>
       </c>
-      <c r="G82" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H82" s="4"/>
-    </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H82" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I82" s="4"/>
+    </row>
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0.7</v>
       </c>
@@ -2770,17 +3149,21 @@
         <v>61.7214651618999</v>
       </c>
       <c r="E83" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.8563009846810159</v>
+      </c>
+      <c r="F83" s="4">
         <v>5.0660245321630404</v>
       </c>
-      <c r="F83" s="4">
+      <c r="G83" s="4">
         <v>49.353049907578502</v>
       </c>
-      <c r="G83" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H83" s="4"/>
-    </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H83" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" s="4"/>
+    </row>
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0.7</v>
       </c>
@@ -2794,17 +3177,21 @@
         <v>63.363847559789598</v>
       </c>
       <c r="E84" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.9601411771267978</v>
+      </c>
+      <c r="F84" s="4">
         <v>5.4849371756276701</v>
       </c>
-      <c r="F84" s="4">
+      <c r="G84" s="4">
         <v>45.471349353049902</v>
       </c>
-      <c r="G84" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H84" s="4"/>
-    </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H84" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I84" s="4"/>
+    </row>
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0.7</v>
       </c>
@@ -2818,17 +3205,21 @@
         <v>66.9500671288002</v>
       </c>
       <c r="E85" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.1823020678046472</v>
+      </c>
+      <c r="F85" s="4">
         <v>5.2985483785026002</v>
       </c>
-      <c r="F85" s="4">
+      <c r="G85" s="4">
         <v>48.2439926062846</v>
       </c>
-      <c r="G85" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H85" s="4"/>
-    </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H85" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I85" s="4"/>
+    </row>
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0.7</v>
       </c>
@@ -2842,17 +3233,21 @@
         <v>81.894378027501702</v>
       </c>
       <c r="E86" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.0495512611124376</v>
+      </c>
+      <c r="F86" s="4">
         <v>5.1084486065488797</v>
       </c>
-      <c r="F86" s="4">
+      <c r="G86" s="4">
         <v>48.983364140480496</v>
       </c>
-      <c r="G86" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H86" s="4"/>
-    </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H86" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I86" s="4"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0.7</v>
       </c>
@@ -2866,17 +3261,21 @@
         <v>57.833443495350203</v>
       </c>
       <c r="E87" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.6048302739344686</v>
+      </c>
+      <c r="F87" s="4">
         <v>4.8732824609055596</v>
       </c>
-      <c r="F87" s="4">
+      <c r="G87" s="4">
         <v>50.831792975970401</v>
       </c>
-      <c r="G87" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H87" s="4"/>
-    </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H87" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I87" s="4"/>
+    </row>
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0.7</v>
       </c>
@@ -2890,17 +3289,21 @@
         <v>66.588556356659197</v>
       </c>
       <c r="E88" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.1601811472944146</v>
+      </c>
+      <c r="F88" s="4">
         <v>4.7208599464915597</v>
       </c>
-      <c r="F88" s="4">
+      <c r="G88" s="4">
         <v>51.940850277264303</v>
       </c>
-      <c r="G88" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H88" s="4"/>
-    </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H88" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I88" s="4"/>
+    </row>
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0.7</v>
       </c>
@@ -2914,17 +3317,21 @@
         <v>80.260546192444096</v>
       </c>
       <c r="E89" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.9588250453083464</v>
+      </c>
+      <c r="F89" s="4">
         <v>5.9788795178155603</v>
       </c>
-      <c r="F89" s="4">
+      <c r="G89" s="4">
         <v>41.219963031423198</v>
       </c>
-      <c r="G89" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H89" s="4"/>
-    </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H89" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I89" s="4"/>
+    </row>
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0.7</v>
       </c>
@@ -2938,17 +3345,21 @@
         <v>86.142398178467204</v>
       </c>
       <c r="E90" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.2812929152390833</v>
+      </c>
+      <c r="F90" s="4">
         <v>5.3440348784756999</v>
       </c>
-      <c r="F90" s="4">
+      <c r="G90" s="4">
         <v>47.504621072088703</v>
       </c>
-      <c r="G90" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H90" s="4"/>
-    </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H90" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I90" s="4"/>
+    </row>
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0.7</v>
       </c>
@@ -2962,17 +3373,21 @@
         <v>65.462656553483498</v>
       </c>
       <c r="E91" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0908996133608966</v>
+      </c>
+      <c r="F91" s="4">
         <v>5.06941961986547</v>
       </c>
-      <c r="F91" s="4">
+      <c r="G91" s="4">
         <v>49.537892791127497</v>
       </c>
-      <c r="G91" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H91" s="4"/>
-    </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H91" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I91" s="4"/>
+    </row>
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0.7</v>
       </c>
@@ -2986,17 +3401,21 @@
         <v>65.585714512964202</v>
       </c>
       <c r="E92" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0985007571132694</v>
+      </c>
+      <c r="F92" s="4">
         <v>4.8618613117377398</v>
       </c>
-      <c r="F92" s="4">
+      <c r="G92" s="4">
         <v>50.646950092421399</v>
       </c>
-      <c r="G92" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H92" s="4"/>
-    </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H92" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I92" s="4"/>
+    </row>
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0.7</v>
       </c>
@@ -3010,17 +3429,21 @@
         <v>61.228771583430202</v>
       </c>
       <c r="E93" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.8248815699300014</v>
+      </c>
+      <c r="F93" s="4">
         <v>5.5084610986584401</v>
       </c>
-      <c r="F93" s="4">
+      <c r="G93" s="4">
         <v>45.656192236598798</v>
       </c>
-      <c r="G93" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H93" s="4"/>
-    </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H93" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I93" s="4"/>
+    </row>
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0.7</v>
       </c>
@@ -3034,17 +3457,21 @@
         <v>76.604952757548006</v>
       </c>
       <c r="E94" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.7524255356756964</v>
+      </c>
+      <c r="F94" s="4">
         <v>5.1019841736438201</v>
       </c>
-      <c r="F94" s="4">
+      <c r="G94" s="4">
         <v>49.537892791127497</v>
       </c>
-      <c r="G94" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H94" s="4"/>
-    </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H94" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I94" s="4"/>
+    </row>
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>0.7</v>
       </c>
@@ -3058,17 +3485,21 @@
         <v>72.560613142143893</v>
       </c>
       <c r="E95" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5182517655997874</v>
+      </c>
+      <c r="F95" s="4">
         <v>5.2610715821731899</v>
       </c>
-      <c r="F95" s="4">
+      <c r="G95" s="4">
         <v>48.2439926062846</v>
       </c>
-      <c r="G95" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H95" s="4"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H95" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I95" s="4"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0.7</v>
       </c>
@@ -3082,17 +3513,21 @@
         <v>56.707078704551897</v>
       </c>
       <c r="E96" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.5304102613703519</v>
+      </c>
+      <c r="F96" s="4">
         <v>4.72412471634021</v>
       </c>
-      <c r="F96" s="4">
+      <c r="G96" s="4">
         <v>52.495378927911197</v>
       </c>
-      <c r="G96" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H96" s="4"/>
-    </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H96" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I96" s="4"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0.7</v>
       </c>
@@ -3106,17 +3541,21 @@
         <v>63.063334988578099</v>
       </c>
       <c r="E97" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.9412426602250417</v>
+      </c>
+      <c r="F97" s="4">
         <v>5.13507743934532</v>
       </c>
-      <c r="F97" s="4">
+      <c r="G97" s="4">
         <v>49.168207024029499</v>
       </c>
-      <c r="G97" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H97" s="4"/>
-    </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H97" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I97" s="4"/>
+    </row>
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0.7</v>
       </c>
@@ -3130,17 +3569,21 @@
         <v>80.340555229821604</v>
       </c>
       <c r="E98" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.963289308608843</v>
+      </c>
+      <c r="F98" s="4">
         <v>5.1672015675435299</v>
       </c>
-      <c r="F98" s="4">
+      <c r="G98" s="4">
         <v>48.7985212569316</v>
       </c>
-      <c r="G98" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H98" s="4"/>
-    </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H98" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I98" s="4"/>
+    </row>
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>0.7</v>
       </c>
@@ -3154,17 +3597,21 @@
         <v>69.282990122458401</v>
       </c>
       <c r="E99" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3236404368796713</v>
+      </c>
+      <c r="F99" s="4">
         <v>5.2658362702695198</v>
       </c>
-      <c r="F99" s="4">
+      <c r="G99" s="4">
         <v>47.689463955637699</v>
       </c>
-      <c r="G99" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H99" s="4"/>
-    </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H99" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I99" s="4"/>
+    </row>
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0.7</v>
       </c>
@@ -3178,17 +3625,21 @@
         <v>64.472128404486796</v>
       </c>
       <c r="E100" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0294538048666055</v>
+      </c>
+      <c r="F100" s="4">
         <v>5.2495011131315099</v>
       </c>
-      <c r="F100" s="4">
+      <c r="G100" s="4">
         <v>47.874306839186602</v>
       </c>
-      <c r="G100" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H100" s="4"/>
-    </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H100" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I100" s="4"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0.7</v>
       </c>
@@ -3202,17 +3653,21 @@
         <v>61.9029143892242</v>
       </c>
       <c r="E101" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.8678405162550291</v>
+      </c>
+      <c r="F101" s="4">
         <v>5.3012194967797699</v>
       </c>
-      <c r="F101" s="4">
+      <c r="G101" s="4">
         <v>46.580406654343797</v>
       </c>
-      <c r="G101" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H101" s="4"/>
-    </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H101" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I101" s="4"/>
+    </row>
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0.8</v>
       </c>
@@ -3226,17 +3681,21 @@
         <v>74.059180310825695</v>
       </c>
       <c r="E102" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.6057643652859621</v>
+      </c>
+      <c r="F102" s="4">
         <v>5.1880207890670196</v>
       </c>
-      <c r="F102" s="4">
+      <c r="G102" s="4">
         <v>48.983364140480496</v>
       </c>
-      <c r="G102" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H102" s="4"/>
-    </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H102" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I102" s="4"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0.8</v>
       </c>
@@ -3250,17 +3709,21 @@
         <v>62.070626080807301</v>
       </c>
       <c r="E103" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.8784913581730418</v>
+      </c>
+      <c r="F103" s="4">
         <v>4.9881251015779098</v>
       </c>
-      <c r="F103" s="4">
+      <c r="G103" s="4">
         <v>50.277264325323401</v>
       </c>
-      <c r="G103" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H103" s="4"/>
-    </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H103" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I103" s="4"/>
+    </row>
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0.8</v>
       </c>
@@ -3274,17 +3737,21 @@
         <v>68.678218855655103</v>
       </c>
       <c r="E104" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2872322795765232</v>
+      </c>
+      <c r="F104" s="4">
         <v>4.9700532341808197</v>
       </c>
-      <c r="F104" s="4">
+      <c r="G104" s="4">
         <v>50.277264325323401</v>
       </c>
-      <c r="G104" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H104" s="4"/>
-    </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H104" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I104" s="4"/>
+    </row>
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0.8</v>
       </c>
@@ -3298,17 +3765,21 @@
         <v>73.990989713263303</v>
       </c>
       <c r="E105" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.6018015388209985</v>
+      </c>
+      <c r="F105" s="4">
         <v>5.4562708536783804</v>
       </c>
-      <c r="F105" s="4">
+      <c r="G105" s="4">
         <v>45.101663585951897</v>
       </c>
-      <c r="G105" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H105" s="4"/>
-    </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H105" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I105" s="4"/>
+    </row>
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0.8</v>
       </c>
@@ -3322,17 +3793,21 @@
         <v>72.321436249174099</v>
       </c>
       <c r="E106" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.504201094116608</v>
+      </c>
+      <c r="F106" s="4">
         <v>4.8662330450146598</v>
       </c>
-      <c r="F106" s="4">
+      <c r="G106" s="4">
         <v>50.831792975970401</v>
       </c>
-      <c r="G106" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H106" s="4"/>
-    </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H106" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I106" s="4"/>
+    </row>
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0.8</v>
       </c>
@@ -3346,17 +3821,21 @@
         <v>70.249785742345395</v>
       </c>
       <c r="E107" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3815145255702674</v>
+      </c>
+      <c r="F107" s="4">
         <v>4.7951986866612497</v>
       </c>
-      <c r="F107" s="4">
+      <c r="G107" s="4">
         <v>51.386321626617303</v>
       </c>
-      <c r="G107" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H107" s="4"/>
-    </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H107" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I107" s="4"/>
+    </row>
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0.8</v>
       </c>
@@ -3370,17 +3849,21 @@
         <v>69.431008224346201</v>
       </c>
       <c r="E108" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3325271211287522</v>
+      </c>
+      <c r="F108" s="4">
         <v>5.1586565580727699</v>
       </c>
-      <c r="F108" s="4">
+      <c r="G108" s="4">
         <v>48.7985212569316</v>
       </c>
-      <c r="G108" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H108" s="4"/>
-    </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H108" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I108" s="4"/>
+    </row>
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0.8</v>
       </c>
@@ -3394,17 +3877,21 @@
         <v>70.837341816279803</v>
       </c>
       <c r="E109" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.4164922513051597</v>
+      </c>
+      <c r="F109" s="4">
         <v>5.2797660081746098</v>
       </c>
-      <c r="F109" s="4">
+      <c r="G109" s="4">
         <v>48.428835489833602</v>
       </c>
-      <c r="G109" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H109" s="4"/>
-    </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H109" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I109" s="4"/>
+    </row>
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0.8</v>
       </c>
@@ -3418,17 +3905,21 @@
         <v>73.351161709995196</v>
       </c>
       <c r="E110" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.564529275447379</v>
+      </c>
+      <c r="F110" s="4">
         <v>5.186619676736</v>
       </c>
-      <c r="F110" s="4">
+      <c r="G110" s="4">
         <v>48.7985212569316</v>
       </c>
-      <c r="G110" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H110" s="4"/>
-    </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H110" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I110" s="4"/>
+    </row>
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0.8</v>
       </c>
@@ -3442,17 +3933,21 @@
         <v>64.987857219251794</v>
       </c>
       <c r="E111" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0615046498313081</v>
+      </c>
+      <c r="F111" s="4">
         <v>4.6184978994704302</v>
       </c>
-      <c r="F111" s="4">
+      <c r="G111" s="4">
         <v>52.6802218114602</v>
       </c>
-      <c r="G111" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H111" s="4"/>
-    </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H111" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I111" s="4"/>
+    </row>
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0.8</v>
       </c>
@@ -3466,17 +3961,21 @@
         <v>63.514764204042898</v>
       </c>
       <c r="E112" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.9696150599663778</v>
+      </c>
+      <c r="F112" s="4">
         <v>4.97710558662481</v>
       </c>
-      <c r="F112" s="4">
+      <c r="G112" s="4">
         <v>50.277264325323401</v>
       </c>
-      <c r="G112" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H112" s="4"/>
-    </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H112" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I112" s="4"/>
+    </row>
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0.8</v>
       </c>
@@ -3490,17 +3989,21 @@
         <v>63.7149858175055</v>
       </c>
       <c r="E113" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.9821667370147997</v>
+      </c>
+      <c r="F113" s="4">
         <v>5.3708027967317804</v>
       </c>
-      <c r="F113" s="4">
+      <c r="G113" s="4">
         <v>47.319778188539701</v>
       </c>
-      <c r="G113" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H113" s="4"/>
-    </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H113" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I113" s="4"/>
+    </row>
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0.8</v>
       </c>
@@ -3514,17 +4017,21 @@
         <v>83.421913880296998</v>
       </c>
       <c r="E114" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.1335597594966771</v>
+      </c>
+      <c r="F114" s="4">
         <v>5.2268568069215799</v>
       </c>
-      <c r="F114" s="4">
+      <c r="G114" s="4">
         <v>47.319778188539701</v>
       </c>
-      <c r="G114" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H114" s="4"/>
-    </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H114" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I114" s="4"/>
+    </row>
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0.8</v>
       </c>
@@ -3538,17 +4045,21 @@
         <v>75.676638957533001</v>
       </c>
       <c r="E115" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.6992320901061717</v>
+      </c>
+      <c r="F115" s="4">
         <v>5.5383638575073704</v>
       </c>
-      <c r="F115" s="4">
+      <c r="G115" s="4">
         <v>46.395563770794801</v>
       </c>
-      <c r="G115" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H115" s="4"/>
-    </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H115" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I115" s="4"/>
+    </row>
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0.8</v>
       </c>
@@ -3562,17 +4073,21 @@
         <v>67.946423119846401</v>
       </c>
       <c r="E116" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2429620355698834</v>
+      </c>
+      <c r="F116" s="4">
         <v>4.8271273656784404</v>
       </c>
-      <c r="F116" s="4">
+      <c r="G116" s="4">
         <v>50.646950092421399</v>
       </c>
-      <c r="G116" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H116" s="4"/>
-    </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H116" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I116" s="4"/>
+    </row>
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>0.8</v>
       </c>
@@ -3586,17 +4101,21 @@
         <v>68.453075782648895</v>
       </c>
       <c r="E117" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2736373973391473</v>
+      </c>
+      <c r="F117" s="4">
         <v>5.4086851410859298</v>
       </c>
-      <c r="F117" s="4">
+      <c r="G117" s="4">
         <v>47.134935304990698</v>
       </c>
-      <c r="G117" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H117" s="4"/>
-    </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H117" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I117" s="4"/>
+    </row>
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0.8</v>
       </c>
@@ -3610,17 +4129,21 @@
         <v>87.000188605401902</v>
       </c>
       <c r="E118" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.3273891633941108</v>
+      </c>
+      <c r="F118" s="4">
         <v>5.3265152713493498</v>
       </c>
-      <c r="F118" s="4">
+      <c r="G118" s="4">
         <v>46.950092421441703</v>
       </c>
-      <c r="G118" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H118" s="4"/>
-    </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H118" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I118" s="4"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0.8</v>
       </c>
@@ -3634,17 +4157,21 @@
         <v>59.044514322897797</v>
       </c>
       <c r="E119" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.6840428371331839</v>
+      </c>
+      <c r="F119" s="4">
         <v>4.9219250300961104</v>
       </c>
-      <c r="F119" s="4">
+      <c r="G119" s="4">
         <v>51.016635859519397</v>
       </c>
-      <c r="G119" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H119" s="4"/>
-    </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H119" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I119" s="4"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0.8</v>
       </c>
@@ -3658,17 +4185,21 @@
         <v>62.624844986497799</v>
       </c>
       <c r="E120" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>7.9135861015406785</v>
+      </c>
+      <c r="F120" s="4">
         <v>4.76347825333879</v>
       </c>
-      <c r="F120" s="4">
+      <c r="G120" s="4">
         <v>51.2014787430683</v>
       </c>
-      <c r="G120" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H120" s="4"/>
-    </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H120" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I120" s="4"/>
+    </row>
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>0.8</v>
       </c>
@@ -3682,17 +4213,21 @@
         <v>65.678010062677799</v>
       </c>
       <c r="E121" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.1041970646497603</v>
+      </c>
+      <c r="F121" s="4">
         <v>5.4540673503725499</v>
       </c>
-      <c r="F121" s="4">
+      <c r="G121" s="4">
         <v>46.580406654343797</v>
       </c>
-      <c r="G121" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H121" s="4"/>
-    </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H121" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I121" s="4"/>
+    </row>
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>0.9</v>
       </c>
@@ -3706,17 +4241,21 @@
         <v>84.869251131350296</v>
       </c>
       <c r="E122" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.2124508753832881</v>
+      </c>
+      <c r="F122" s="4">
         <v>5.6626456811362198</v>
       </c>
-      <c r="F122" s="4">
+      <c r="G122" s="4">
         <v>45.2865064695009</v>
       </c>
-      <c r="G122" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H122" s="4"/>
-    </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H122" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I122" s="4"/>
+    </row>
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>0.9</v>
       </c>
@@ -3730,17 +4269,21 @@
         <v>68.096656559575706</v>
       </c>
       <c r="E123" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.2520698348702624</v>
+      </c>
+      <c r="F123" s="4">
         <v>4.8972842513295003</v>
       </c>
-      <c r="F123" s="4">
+      <c r="G123" s="4">
         <v>50.831792975970401</v>
       </c>
-      <c r="G123" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H123" s="4"/>
-    </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H123" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I123" s="4"/>
+    </row>
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>0.9</v>
       </c>
@@ -3754,17 +4297,21 @@
         <v>64.4878191992007</v>
       </c>
       <c r="E124" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0304308227641616</v>
+      </c>
+      <c r="F124" s="4">
         <v>5.2254875142087096</v>
       </c>
-      <c r="F124" s="4">
+      <c r="G124" s="4">
         <v>48.428835489833602</v>
       </c>
-      <c r="G124" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H124" s="4"/>
-    </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H124" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I124" s="4"/>
+    </row>
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>0.9</v>
       </c>
@@ -3778,17 +4325,21 @@
         <v>69.628942845709403</v>
       </c>
       <c r="E125" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3443958945935321</v>
+      </c>
+      <c r="F125" s="4">
         <v>5.4991686933937798</v>
       </c>
-      <c r="F125" s="4">
+      <c r="G125" s="4">
         <v>45.841035120147801</v>
       </c>
-      <c r="G125" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H125" s="4"/>
-    </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H125" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I125" s="4"/>
+    </row>
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0.9</v>
       </c>
@@ -3802,17 +4353,21 @@
         <v>86.415585487915706</v>
       </c>
       <c r="E126" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.2959983588593484</v>
+      </c>
+      <c r="F126" s="4">
         <v>5.3038009007771798</v>
       </c>
-      <c r="F126" s="4">
+      <c r="G126" s="4">
         <v>46.210720887245799</v>
       </c>
-      <c r="G126" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H126" s="4"/>
-    </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H126" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I126" s="4"/>
+    </row>
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>0.9</v>
       </c>
@@ -3826,17 +4381,21 @@
         <v>74.047010023360301</v>
       </c>
       <c r="E127" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.6050572353332022</v>
+      </c>
+      <c r="F127" s="4">
         <v>5.2722833493004497</v>
       </c>
-      <c r="F127" s="4">
+      <c r="G127" s="4">
         <v>47.874306839186602</v>
       </c>
-      <c r="G127" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H127" s="4"/>
-    </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H127" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I127" s="4"/>
+    </row>
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>0.9</v>
       </c>
@@ -3850,17 +4409,21 @@
         <v>64.4191740885679</v>
       </c>
       <c r="E128" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.0261556232462805</v>
+      </c>
+      <c r="F128" s="4">
         <v>4.9481753393112502</v>
       </c>
-      <c r="F128" s="4">
+      <c r="G128" s="4">
         <v>50.277264325323401</v>
       </c>
-      <c r="G128" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H128" s="4"/>
-    </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H128" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I128" s="4"/>
+    </row>
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>0.9</v>
       </c>
@@ -3874,17 +4437,21 @@
         <v>72.656001967114506</v>
       </c>
       <c r="E129" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5238490112809071</v>
+      </c>
+      <c r="F129" s="4">
         <v>5.4602980180220104</v>
       </c>
-      <c r="F129" s="4">
+      <c r="G129" s="4">
         <v>47.134935304990698</v>
       </c>
-      <c r="G129" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H129" s="4"/>
-    </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H129" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I129" s="4"/>
+    </row>
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>0.9</v>
       </c>
@@ -3898,17 +4465,21 @@
         <v>92.414648031351007</v>
       </c>
       <c r="E130" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.6132537692162803</v>
+      </c>
+      <c r="F130" s="4">
         <v>5.5799854543725003</v>
       </c>
-      <c r="F130" s="4">
+      <c r="G130" s="4">
         <v>46.395563770794801</v>
       </c>
-      <c r="G130" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H130" s="4"/>
-    </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H130" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I130" s="4"/>
+    </row>
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>0.9</v>
       </c>
@@ -3922,17 +4493,21 @@
         <v>76.667057552090796</v>
       </c>
       <c r="E131" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.7559726788113501</v>
+      </c>
+      <c r="F131" s="4">
         <v>5.2449332409731797</v>
       </c>
-      <c r="F131" s="4">
+      <c r="G131" s="4">
         <v>48.2439926062846</v>
       </c>
-      <c r="G131" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H131" s="4"/>
-    </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H131" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I131" s="4"/>
+    </row>
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>0.9</v>
       </c>
@@ -3946,17 +4521,21 @@
         <v>71.744670691639996</v>
       </c>
       <c r="E132" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.4702225880811426</v>
+      </c>
+      <c r="F132" s="4">
         <v>5.3057020947449196</v>
       </c>
-      <c r="F132" s="4">
+      <c r="G132" s="4">
         <v>46.580406654343797</v>
       </c>
-      <c r="G132" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H132" s="4"/>
-    </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H132" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I132" s="4"/>
+    </row>
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>0.9</v>
       </c>
@@ -3970,17 +4549,21 @@
         <v>70.930025858711602</v>
       </c>
       <c r="E133" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.4219965482486163</v>
+      </c>
+      <c r="F133" s="4">
         <v>5.3587842101621499</v>
       </c>
-      <c r="F133" s="4">
+      <c r="G133" s="4">
         <v>45.656192236598798</v>
       </c>
-      <c r="G133" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H133" s="4"/>
-    </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H133" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I133" s="4"/>
+    </row>
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>0.9</v>
       </c>
@@ -3994,17 +4577,21 @@
         <v>101.458011394507</v>
       </c>
       <c r="E134" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>10.072636764745713</v>
+      </c>
+      <c r="F134" s="4">
         <v>5.52933022965356</v>
       </c>
-      <c r="F134" s="4">
+      <c r="G134" s="4">
         <v>46.025878003696803</v>
       </c>
-      <c r="G134" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H134" s="4"/>
-    </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H134" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I134" s="4"/>
+    </row>
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>0.9</v>
       </c>
@@ -4018,17 +4605,21 @@
         <v>81.4630189708773</v>
       </c>
       <c r="E135" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.025686620467015</v>
+      </c>
+      <c r="F135" s="4">
         <v>4.7748881253329101</v>
       </c>
-      <c r="F135" s="4">
+      <c r="G135" s="4">
         <v>51.571164510166298</v>
       </c>
-      <c r="G135" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H135" s="4"/>
-    </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H135" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I135" s="4"/>
+    </row>
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>0.9</v>
       </c>
@@ -4042,17 +4633,21 @@
         <v>68.942589440760003</v>
       </c>
       <c r="E136" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3031674342241235</v>
+      </c>
+      <c r="F136" s="4">
         <v>5.0918659353512101</v>
       </c>
-      <c r="F136" s="4">
+      <c r="G136" s="4">
         <v>49.168207024029499</v>
       </c>
-      <c r="G136" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H136" s="4"/>
-    </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H136" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I136" s="4"/>
+    </row>
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>0.9</v>
       </c>
@@ -4066,17 +4661,21 @@
         <v>72.483340927941896</v>
       </c>
       <c r="E137" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5137148723657585</v>
+      </c>
+      <c r="F137" s="4">
         <v>5.7168452707233497</v>
       </c>
-      <c r="F137" s="4">
+      <c r="G137" s="4">
         <v>42.883548983364101</v>
       </c>
-      <c r="G137" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H137" s="4"/>
-    </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H137" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I137" s="4"/>
+    </row>
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>0.9</v>
       </c>
@@ -4090,17 +4689,21 @@
         <v>87.026733215106304</v>
       </c>
       <c r="E138" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>9.3288119937699623</v>
+      </c>
+      <c r="F138" s="4">
         <v>5.5960653948165398</v>
       </c>
-      <c r="F138" s="4">
+      <c r="G138" s="4">
         <v>43.438077634011002</v>
       </c>
-      <c r="G138" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H138" s="4"/>
-    </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H138" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I138" s="4"/>
+    </row>
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>0.9</v>
       </c>
@@ -4114,17 +4717,21 @@
         <v>69.218666161274498</v>
       </c>
       <c r="E139" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.3197756076275571</v>
+      </c>
+      <c r="F139" s="4">
         <v>4.6119188535011402</v>
       </c>
-      <c r="F139" s="4">
+      <c r="G139" s="4">
         <v>53.419593345656097</v>
       </c>
-      <c r="G139" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H139" s="4"/>
-    </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H139" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I139" s="4"/>
+    </row>
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>0.9</v>
       </c>
@@ -4138,17 +4745,21 @@
         <v>72.4125418107743</v>
       </c>
       <c r="E140" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.5095559114899935</v>
+      </c>
+      <c r="F140" s="4">
         <v>5.1765987998560901</v>
       </c>
-      <c r="F140" s="4">
+      <c r="G140" s="4">
         <v>47.874306839186602</v>
       </c>
-      <c r="G140" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H140" s="4"/>
-    </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H140" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I140" s="4"/>
+    </row>
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>0.9</v>
       </c>
@@ -4162,15 +4773,19 @@
         <v>66.691591837489895</v>
       </c>
       <c r="E141" s="4">
+        <f>SQRT(Table1[[#This Row],[Loss]])</f>
+        <v>8.1664920153937519</v>
+      </c>
+      <c r="F141" s="4">
         <v>5.3416884586289601</v>
       </c>
-      <c r="F141" s="4">
+      <c r="G141" s="4">
         <v>47.134935304990698</v>
       </c>
-      <c r="G141" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H141" s="4"/>
+      <c r="H141" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I141" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>